<commit_message>
finished another fair comparison
</commit_message>
<xml_diff>
--- a/algorithm/amplitude_comparison/amplitude_comparison_stats_mix.xlsx
+++ b/algorithm/amplitude_comparison/amplitude_comparison_stats_mix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Note_Database\Subject\MS Monographic Study\MS Phase6\MCU\SMRBS-ESP32\algorithm\amplitude_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C60E1E6-5BB4-45EB-A9C5-2BB7CFFDA96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F1E162-398F-413A-8C5A-29467C04BFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,10 +57,6 @@
   </si>
   <si>
     <t>max</t>
-  </si>
-  <si>
-    <t>compensation</t>
-    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>max</t>
@@ -112,6 +108,10 @@
   </si>
   <si>
     <t>mid6</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>scale</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -506,7 +506,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -522,25 +522,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
@@ -553,12 +538,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
@@ -746,22 +725,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.3475889999999999</c:v>
+                  <c:v>1.44047709497207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.487436</c:v>
+                  <c:v>1.6084152173913</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.412528</c:v>
+                  <c:v>1.7151907654920999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6994229999999999</c:v>
+                  <c:v>2.0797431761786598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.85933300000000001</c:v>
+                  <c:v>2.1275547263681598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.529416</c:v>
+                  <c:v>1.3647974025973999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -803,22 +782,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.61851206233205402</c:v>
+                  <c:v>0.156994960236467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56401748521444595</c:v>
+                  <c:v>0.32530622617931898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74519002099020604</c:v>
+                  <c:v>0.39586748662978299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96972746038173996</c:v>
+                  <c:v>0.330158305408778</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.07211225008755</c:v>
+                  <c:v>0.406280418914162</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66905493305665698</c:v>
+                  <c:v>0.159139517187705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,22 +839,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.0669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>1.1060000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.274</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.486</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.085</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,22 +896,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.296</c:v>
+                  <c:v>1.3445</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3987499999999999</c:v>
+                  <c:v>1.4157500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.444</c:v>
+                  <c:v>1.4910000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6665000000000001</c:v>
+                  <c:v>1.9339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>1.8022499999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,22 +953,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.4145000000000001</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4715</c:v>
+                  <c:v>1.4815</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.52</c:v>
+                  <c:v>1.544</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.96</c:v>
+                  <c:v>1.984</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>1.8979999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>1.3879999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1031,22 +1010,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.5322499999999999</c:v>
+                  <c:v>1.5449999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5649999999999999</c:v>
+                  <c:v>1.5765</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5960000000000001</c:v>
+                  <c:v>1.6160000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0262500000000001</c:v>
+                  <c:v>2.0467499999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8380000000000001</c:v>
+                  <c:v>2.6287500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.23725</c:v>
+                  <c:v>1.5129999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1090,16 +1069,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.084</c:v>
+                  <c:v>1.927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2779999999999996</c:v>
+                  <c:v>2.4260000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.6970000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.096</c:v>
+                  <c:v>2.9740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.8959999999999999</c:v>
@@ -1546,22 +1525,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.3475889999999999</c:v>
+                  <c:v>1.44047709497207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.487436</c:v>
+                  <c:v>1.6084152173913</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.412528</c:v>
+                  <c:v>1.7151907654920999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6994229999999999</c:v>
+                  <c:v>2.0797431761786598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.85933300000000001</c:v>
+                  <c:v>2.1275547263681598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.529416</c:v>
+                  <c:v>1.3647974025973999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1605,22 +1584,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.61851206233205402</c:v>
+                  <c:v>0.156994960236467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56401748521444595</c:v>
+                  <c:v>0.32530622617931898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74519002099020604</c:v>
+                  <c:v>0.39586748662978299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96972746038173996</c:v>
+                  <c:v>0.330158305408778</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.07211225008755</c:v>
+                  <c:v>0.406280418914162</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66905493305665698</c:v>
+                  <c:v>0.159139517187705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1664,22 +1643,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.0669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>1.1060000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.274</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.486</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.085</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1723,22 +1702,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.296</c:v>
+                  <c:v>1.3445</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3987499999999999</c:v>
+                  <c:v>1.4157500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.444</c:v>
+                  <c:v>1.4910000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6665000000000001</c:v>
+                  <c:v>1.9339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>1.8022499999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1782,22 +1761,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.4145000000000001</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4715</c:v>
+                  <c:v>1.4815</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.52</c:v>
+                  <c:v>1.544</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.96</c:v>
+                  <c:v>1.984</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>1.8979999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>1.3879999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1841,22 +1820,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.5322499999999999</c:v>
+                  <c:v>1.5449999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5649999999999999</c:v>
+                  <c:v>1.5765</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5960000000000001</c:v>
+                  <c:v>1.6160000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0262500000000001</c:v>
+                  <c:v>2.0467499999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8380000000000001</c:v>
+                  <c:v>2.6287500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.23725</c:v>
+                  <c:v>1.5129999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1902,16 +1881,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.084</c:v>
+                  <c:v>1.927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2779999999999996</c:v>
+                  <c:v>2.4260000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.6970000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.096</c:v>
+                  <c:v>2.9740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.8959999999999999</c:v>
@@ -6501,8 +6480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6513,121 +6492,121 @@
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="8">
+        <v>895</v>
+      </c>
+      <c r="C2" s="9">
+        <v>920</v>
+      </c>
+      <c r="D2" s="9">
+        <v>823</v>
+      </c>
+      <c r="E2" s="9">
+        <v>806</v>
+      </c>
+      <c r="F2" s="9">
+        <v>402</v>
+      </c>
+      <c r="G2" s="20">
+        <v>385</v>
+      </c>
+      <c r="H2" s="18">
         <v>1000</v>
       </c>
-      <c r="C2" s="14">
+      <c r="I2" s="9">
         <v>1000</v>
       </c>
-      <c r="D2" s="14">
+      <c r="J2" s="9">
         <v>1000</v>
       </c>
-      <c r="E2" s="14">
+      <c r="K2" s="9">
         <v>1000</v>
       </c>
-      <c r="F2" s="14">
+      <c r="L2" s="9">
         <v>1000</v>
       </c>
-      <c r="G2" s="27">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="25">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J2" s="14">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="14">
-        <v>1000</v>
-      </c>
-      <c r="L2" s="14">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="15">
+      <c r="M2" s="10">
         <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16">
-        <v>1.3475889999999999</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1.487436</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1.412528</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1.6994229999999999</v>
-      </c>
-      <c r="F3" s="10">
-        <v>0.85933300000000001</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0.529416</v>
-      </c>
-      <c r="H3" s="9">
+      <c r="B3" s="11">
+        <v>1.44047709497207</v>
+      </c>
+      <c r="C3">
+        <v>1.6084152173913</v>
+      </c>
+      <c r="D3">
+        <v>1.7151907654920999</v>
+      </c>
+      <c r="E3">
+        <v>2.0797431761786598</v>
+      </c>
+      <c r="F3">
+        <v>2.1275547263681598</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.3647974025973999</v>
+      </c>
+      <c r="H3" s="6">
         <v>-6.8349999999999999E-3</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3">
         <v>-4.8479999999999999E-3</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3">
         <v>-8.0040000000000007E-3</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3">
         <v>-1.9191E-2</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3">
         <v>-1.05E-4</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="12">
         <v>-1.0020000000000001E-3</v>
       </c>
     </row>
@@ -6635,40 +6614,40 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18">
-        <v>0.61851206233205402</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0.56401748521444595</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.74519002099020604</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0.96972746038173996</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1.07211225008755</v>
+      <c r="B4" s="11">
+        <v>0.156994960236467</v>
+      </c>
+      <c r="C4">
+        <v>0.32530622617931898</v>
+      </c>
+      <c r="D4">
+        <v>0.39586748662978299</v>
+      </c>
+      <c r="E4">
+        <v>0.330158305408778</v>
+      </c>
+      <c r="F4">
+        <v>0.406280418914162</v>
       </c>
       <c r="G4" s="2">
-        <v>0.66905493305665698</v>
+        <v>0.159139517187705</v>
       </c>
       <c r="H4" s="6">
         <v>0.39696319924717999</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4">
         <v>0.19123093935911101</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4">
         <v>6.8609425279893096E-2</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4">
         <v>0.43401486082669799</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4">
         <v>8.3636864480324105E-2</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="12">
         <v>4.2960442218343102E-2</v>
       </c>
     </row>
@@ -6676,40 +6655,40 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18">
-        <v>2E-3</v>
-      </c>
-      <c r="C5" s="7">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D5" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E5" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F5" s="7">
-        <v>2E-3</v>
+      <c r="B5" s="11">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="D5">
+        <v>1.274</v>
+      </c>
+      <c r="E5">
+        <v>1.486</v>
+      </c>
+      <c r="F5">
+        <v>1.571</v>
       </c>
       <c r="G5" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>1.085</v>
       </c>
       <c r="H5" s="6">
         <v>-8.86</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5">
         <v>-5.7160000000000002</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5">
         <v>-0.249</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5">
         <v>-11.48</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5">
         <v>-0.93</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="12">
         <v>-0.25800000000000001</v>
       </c>
     </row>
@@ -6717,40 +6696,40 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18">
-        <v>1.296</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1.3987499999999999</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1.444</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1.6665000000000001</v>
-      </c>
-      <c r="F6" s="7">
-        <v>5.0000000000000001E-3</v>
+      <c r="B6" s="11">
+        <v>1.3445</v>
+      </c>
+      <c r="C6">
+        <v>1.4157500000000001</v>
+      </c>
+      <c r="D6">
+        <v>1.4910000000000001</v>
+      </c>
+      <c r="E6">
+        <v>1.9339999999999999</v>
+      </c>
+      <c r="F6">
+        <v>1.8022499999999999</v>
       </c>
       <c r="G6" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>1.21</v>
       </c>
       <c r="H6" s="6">
         <v>-4.8000000000000001E-2</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6">
         <v>-3.6999999999999998E-2</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6">
         <v>-0.05</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6">
         <v>-0.03</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="12">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
@@ -6758,64 +6737,64 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="18">
-        <v>1.4145000000000001</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1.4715</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1.52</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1.96</v>
-      </c>
-      <c r="F7" s="7">
-        <v>6.0000000000000001E-3</v>
+      <c r="B7" s="11">
+        <v>1.43</v>
+      </c>
+      <c r="C7">
+        <v>1.4815</v>
+      </c>
+      <c r="D7">
+        <v>1.544</v>
+      </c>
+      <c r="E7">
+        <v>1.984</v>
+      </c>
+      <c r="F7">
+        <v>1.8979999999999999</v>
       </c>
       <c r="G7" s="2">
-        <v>6.0000000000000001E-3</v>
+        <v>1.3879999999999999</v>
       </c>
       <c r="H7" s="6">
         <v>-2E-3</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7">
         <v>-1E-3</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7">
         <v>-1E-3</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7">
         <v>-2E-3</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="12">
         <v>-1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="20">
-        <v>1.5322499999999999</v>
+      <c r="B8" s="13">
+        <v>1.5449999999999999</v>
       </c>
       <c r="C8" s="5">
-        <v>1.5649999999999999</v>
+        <v>1.5765</v>
       </c>
       <c r="D8" s="5">
-        <v>1.5960000000000001</v>
+        <v>1.6160000000000001</v>
       </c>
       <c r="E8" s="5">
-        <v>2.0262500000000001</v>
+        <v>2.0467499999999998</v>
       </c>
       <c r="F8" s="5">
-        <v>1.8380000000000001</v>
+        <v>2.6287500000000001</v>
       </c>
       <c r="G8" s="3">
-        <v>1.23725</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="H8" s="4">
         <v>3.925E-2</v>
@@ -6832,7 +6811,7 @@
       <c r="L8" s="5">
         <v>1E-3</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="14">
         <v>1E-3</v>
       </c>
     </row>
@@ -6840,40 +6819,40 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="22">
-        <v>10.084</v>
-      </c>
-      <c r="C9" s="23">
-        <v>7.2779999999999996</v>
-      </c>
-      <c r="D9" s="23">
+      <c r="B9" s="15">
+        <v>1.927</v>
+      </c>
+      <c r="C9" s="16">
+        <v>2.4260000000000002</v>
+      </c>
+      <c r="D9" s="16">
         <v>2.6970000000000001</v>
       </c>
-      <c r="E9" s="23">
-        <v>13.096</v>
-      </c>
-      <c r="F9" s="23">
+      <c r="E9" s="16">
+        <v>2.9740000000000002</v>
+      </c>
+      <c r="F9" s="16">
         <v>2.8959999999999999</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="21">
         <v>1.7010000000000001</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="19">
         <v>7.7480000000000002</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="16">
         <v>0.34200000000000003</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="16">
         <v>0.57099999999999995</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="16">
         <v>0.21199999999999999</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="16">
         <v>1.5649999999999999</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="17">
         <v>0.76900000000000002</v>
       </c>
     </row>
@@ -6883,31 +6862,31 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <f>MAX(B8:G8)</f>
-        <v>2.0262500000000001</v>
+        <f>MAX(B3:G3)</f>
+        <v>2.1275547263681598</v>
       </c>
       <c r="C11">
-        <f>MAX(B8:G8)</f>
-        <v>2.0262500000000001</v>
+        <f>MAX(B3:G3)</f>
+        <v>2.1275547263681598</v>
       </c>
       <c r="D11">
-        <f>MAX(B8:G8)</f>
-        <v>2.0262500000000001</v>
+        <f>MAX(B3:G3)</f>
+        <v>2.1275547263681598</v>
       </c>
       <c r="E11">
-        <f>MAX(B8:G8)</f>
-        <v>2.0262500000000001</v>
+        <f>MAX(B3:G3)</f>
+        <v>2.1275547263681598</v>
       </c>
       <c r="F11">
-        <f>MAX(B8:G8)</f>
-        <v>2.0262500000000001</v>
+        <f>MAX(B3:G3)</f>
+        <v>2.1275547263681598</v>
       </c>
       <c r="G11" s="2">
-        <f>MAX(B8:G8)</f>
-        <v>2.0262500000000001</v>
+        <f>MAX(B3:G3)</f>
+        <v>2.1275547263681598</v>
       </c>
       <c r="H11" s="6">
         <f>MAX(H8:M8)</f>
@@ -6936,54 +6915,54 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <f>B11/B8</f>
-        <v>1.3224016968510361</v>
+        <f>B11/B3</f>
+        <v>1.4769792132025619</v>
       </c>
       <c r="C12">
-        <f>C11/C8</f>
-        <v>1.2947284345047925</v>
+        <f t="shared" ref="C12:G12" si="0">C11/C3</f>
+        <v>1.322764609140453</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:M12" si="0">D11/D8</f>
-        <v>1.2695802005012531</v>
+        <f t="shared" si="0"/>
+        <v>1.2404187156160147</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.022989160746929</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>1.1024211099020675</v>
-      </c>
-      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>1.6377045867852094</v>
+        <v>1.5588795247698495</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D12:M12" si="1">H11/H8</f>
         <v>1</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.060810810810811</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2265625</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3083333333333333</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.25</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.25</v>
       </c>
     </row>

</xml_diff>